<commit_message>
update hayabusa(1st) return year
はやぶさ帰還9周年に変更（変更漏れていた分は先回りして来年の10周年に直した）
</commit_message>
<xml_diff>
--- a/tweetlist.xlsx
+++ b/tweetlist.xlsx
@@ -3846,23 +3846,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t xml:space="preserve">【お帰りはやぶさ・帰還8周年】6/9 12:30-15:00 最後の軌道修正となるTCM-4完了。4/4-6、5/1-4、5/23-27、6/3-5とあわせ5回の軌道修正でオーストラリア・ウーメラ砂漠の着陸地点へ誘導完了 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">【お帰りはやぶさ・帰還8周年】6/13 19:54 イトカワのサンプルを格納したカプセルの切り離しに成功 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">【お帰りはやぶさ・帰還8周年】6/13 22:51 はやぶさ、地球大気圏再突入。22:56にカプセルからパラシュートが展開され、23:08に着陸を果たした。 </t>
-  </si>
-  <si>
-    <t>【お帰りはやぶさ・帰還8周年】6/13 22:02 はやぶさ、最後の地球撮影。この写真 http://www.isas.jaxa.jp/j/topics/topics/2010/0618_3.shtml を内之浦局に送信中に、内之浦の水平線の向こう側に入り通信途絶(22:28)</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t xml:space="preserve">【お帰りはやぶさ・帰還8周年】6/13 22:28 はやぶさ、内之浦局の観測圏外になり通信途絶。最後の信号はhttp://hayabusa.jaxa.jp/message/message_049.htmlに掲載されている </t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>【今日の人工衛星】2/23 1977年：きく2号 日本初の静止衛星。きくシリーズは技術試験衛星。</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -3900,6 +3883,26 @@
     <rPh sb="97" eb="99">
       <t>テイシ</t>
     </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">【お帰りはやぶさ・帰還10周年】6/9 12:30-15:00 最後の軌道修正となるTCM-4完了。4/4-6、5/1-4、5/23-27、6/3-5とあわせ5回の軌道修正でオーストラリア・ウーメラ砂漠の着陸地点へ誘導完了 </t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">【お帰りはやぶさ・帰還9周年】6/13 19:54 イトカワのサンプルを格納したカプセルの切り離しに成功 </t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>【お帰りはやぶさ・帰還9周年】6/13 22:02 はやぶさ、最後の地球撮影。この写真 http://www.isas.jaxa.jp/j/topics/topics/2010/0618_3.shtml を内之浦局に送信中に、内之浦の水平線の向こう側に入り通信途絶(22:28)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">【お帰りはやぶさ・帰還9周年】6/13 22:28 はやぶさ、内之浦局の観測圏外になり通信途絶。最後の信号はhttp://hayabusa.jaxa.jp/message/message_049.htmlに掲載されている </t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">【お帰りはやぶさ・帰還9周年】6/13 22:51 はやぶさ、地球大気圏再突入。22:56にカプセルからパラシュートが展開され、23:08に着陸を果たした。 </t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -4262,8 +4265,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E531"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A524" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B529" sqref="B529"/>
+    <sheetView tabSelected="1" topLeftCell="A247" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B261" sqref="B261"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -5634,7 +5637,7 @@
         <v>599</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>1062</v>
+        <v>1057</v>
       </c>
       <c r="C112">
         <f t="shared" si="1"/>
@@ -5643,10 +5646,10 @@
     </row>
     <row r="113" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
-        <v>1063</v>
+        <v>1058</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>1065</v>
+        <v>1060</v>
       </c>
       <c r="C113">
         <f t="shared" ref="C113" si="2">LEN(B113)</f>
@@ -5658,7 +5661,7 @@
         <v>600</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>1064</v>
+        <v>1059</v>
       </c>
       <c r="C114">
         <f t="shared" si="1"/>
@@ -7362,14 +7365,14 @@
         <v>733</v>
       </c>
       <c r="B250" s="2" t="s">
-        <v>1057</v>
+        <v>1061</v>
       </c>
       <c r="C250">
         <f t="shared" si="4"/>
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D250">
-        <v>20180608</v>
+        <v>20190610</v>
       </c>
       <c r="E250" t="s">
         <v>1029</v>
@@ -7458,14 +7461,14 @@
         <v>740</v>
       </c>
       <c r="B257" s="2" t="s">
-        <v>1058</v>
+        <v>1062</v>
       </c>
       <c r="C257">
         <f t="shared" si="4"/>
         <v>53</v>
       </c>
       <c r="D257">
-        <v>20180608</v>
+        <v>20190610</v>
       </c>
       <c r="E257" t="s">
         <v>1029</v>
@@ -7476,14 +7479,14 @@
         <v>741</v>
       </c>
       <c r="B258" s="2" t="s">
-        <v>1060</v>
+        <v>1063</v>
       </c>
       <c r="C258">
         <f t="shared" si="4"/>
         <v>139</v>
       </c>
       <c r="D258">
-        <v>20180608</v>
+        <v>20190610</v>
       </c>
       <c r="E258" t="s">
         <v>1029</v>
@@ -7494,14 +7497,14 @@
         <v>742</v>
       </c>
       <c r="B259" s="2" t="s">
-        <v>1061</v>
+        <v>1064</v>
       </c>
       <c r="C259">
         <f t="shared" ref="C259:C322" si="5">LEN(B259)</f>
         <v>111</v>
       </c>
       <c r="D259">
-        <v>20180608</v>
+        <v>20190610</v>
       </c>
       <c r="E259" t="s">
         <v>1029</v>
@@ -7512,14 +7515,14 @@
         <v>743</v>
       </c>
       <c r="B260" s="2" t="s">
-        <v>1059</v>
+        <v>1065</v>
       </c>
       <c r="C260">
         <f t="shared" si="5"/>
         <v>79</v>
       </c>
       <c r="D260">
-        <v>20180608</v>
+        <v>20190610</v>
       </c>
       <c r="E260" t="s">
         <v>1029</v>

</xml_diff>

<commit_message>
fix tweetlist and change Twitter API to v2
</commit_message>
<xml_diff>
--- a/tweetlist.xlsx
+++ b/tweetlist.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\garmy\Documents\GitHub\todayssatellite\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35A39092-EC00-425B-A22D-82D0B6BDFEDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{314EE78B-16E1-44BD-B463-5AB06BAB3F94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1320" yWindow="735" windowWidth="14430" windowHeight="14595" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1140" yWindow="1320" windowWidth="14430" windowHeight="14595" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="todayssatellite" sheetId="1" r:id="rId1"/>
@@ -4127,10 +4127,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t xml:space="preserve">【お帰りはやぶさ・帰還13周年】6/13 22:28 はやぶさ、内之浦局の観測圏外になり通信途絶。最後の信号はhttps://hayabusa.jaxa.jp/message/message_049.htmlに掲載されている </t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>【お帰りはやぶさ・帰還13周年】6/13 22:02 はやぶさ、最後の地球撮影。この写真 https://www.isas.jaxa.jp/j/topics/topics/2010/0618_3.shtml を内之浦局に送信中に内之浦の水平線の向こう側に入り通信途絶(22:28)</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -4143,6 +4139,10 @@
     <rPh sb="3" eb="6">
       <t>セイキカ</t>
     </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">【お帰りはやぶさ・帰還13周年】6/13 22:28 はやぶさ、内之浦局の観測圏外になり通信途絶。最後の信号はhttps://hayabusa.jaxa.jp/message/message_049.html に掲載されている </t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -4492,8 +4492,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G537"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A247" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B256" sqref="B256"/>
+    <sheetView tabSelected="1" topLeftCell="A380" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B390" sqref="B390"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -7745,7 +7745,7 @@
         <v>737</v>
       </c>
       <c r="B260" s="2" t="s">
-        <v>1078</v>
+        <v>1077</v>
       </c>
       <c r="C260">
         <f t="shared" si="4"/>
@@ -7763,14 +7763,14 @@
         <v>738</v>
       </c>
       <c r="B261" s="2" t="s">
-        <v>1077</v>
+        <v>1080</v>
       </c>
       <c r="C261">
         <f t="shared" ref="C261:C324" si="6">LEN(B261)</f>
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D261">
-        <v>20230610</v>
+        <v>20230613</v>
       </c>
       <c r="E261" t="s">
         <v>1025</v>
@@ -10812,7 +10812,7 @@
         <v>974</v>
       </c>
       <c r="B505" s="2" t="s">
-        <v>1079</v>
+        <v>1078</v>
       </c>
       <c r="C505">
         <f t="shared" si="9"/>
@@ -10822,7 +10822,7 @@
         <v>20230609</v>
       </c>
       <c r="E505" t="s">
-        <v>1080</v>
+        <v>1079</v>
       </c>
     </row>
     <row r="506" spans="1:7" ht="40.5" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
update description XRISM, SLIM
</commit_message>
<xml_diff>
--- a/tweetlist.xlsx
+++ b/tweetlist.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98BE6FCB-38EE-4E39-9268-B368000168B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C3D3C36-B5DF-47D3-A419-B8AEE146367B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="21330" yWindow="9360" windowWidth="22350" windowHeight="15045" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -6854,10 +6854,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>【今日の人工衛星】8/27 2023年：X線天文衛星代替機(XRISM)、小型月着陸実証機(SLIM)が打ち上げられました。</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>01/20 00:20:00</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -6963,6 +6959,58 @@
     </rPh>
     <rPh sb="96" eb="97">
       <t>メ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>【今日の人工衛星】8/27 2023年：X線天文衛星代替機(XRISM)、小型月着陸実証機(SLIM) XRISMは、喪失したASTRO-Hの代替機として、期待された科学的成果を上げている。SLIMは、日本発の月面探査機として、ピンポイント着陸を含む様々な世界初の成果を上げた。</t>
+    <rPh sb="59" eb="61">
+      <t>ソウシツ</t>
+    </rPh>
+    <rPh sb="71" eb="74">
+      <t>ダイタイキ</t>
+    </rPh>
+    <rPh sb="78" eb="80">
+      <t>キタイ</t>
+    </rPh>
+    <rPh sb="83" eb="86">
+      <t>カガクテキ</t>
+    </rPh>
+    <rPh sb="86" eb="88">
+      <t>セイカ</t>
+    </rPh>
+    <rPh sb="89" eb="90">
+      <t>ア</t>
+    </rPh>
+    <rPh sb="101" eb="103">
+      <t>ニホン</t>
+    </rPh>
+    <rPh sb="103" eb="104">
+      <t>ハツ</t>
+    </rPh>
+    <rPh sb="105" eb="107">
+      <t>ゲツメン</t>
+    </rPh>
+    <rPh sb="107" eb="110">
+      <t>タンサキ</t>
+    </rPh>
+    <rPh sb="120" eb="122">
+      <t>チャクリク</t>
+    </rPh>
+    <rPh sb="123" eb="124">
+      <t>フク</t>
+    </rPh>
+    <rPh sb="125" eb="127">
+      <t>サマザマ</t>
+    </rPh>
+    <rPh sb="128" eb="131">
+      <t>セカイハツ</t>
+    </rPh>
+    <rPh sb="132" eb="134">
+      <t>セイカ</t>
+    </rPh>
+    <rPh sb="135" eb="136">
+      <t>ア</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -7085,7 +7133,7 @@
   <cellStyles count="1">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="36">
+  <dxfs count="34">
     <dxf>
       <fill>
         <patternFill>
@@ -7213,18 +7261,6 @@
         <name val="游ゴシック"/>
         <family val="3"/>
         <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="游ゴシック"/>
-        <family val="3"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="10"/>
       </font>
     </dxf>
     <dxf>
@@ -11684,16 +11720,16 @@
     <dataField name="個数 / Number" fld="0" subtotal="count" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="32">
-    <format dxfId="35">
+    <format dxfId="33">
       <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="34">
+    <format dxfId="32">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="33">
+    <format dxfId="31">
       <pivotArea field="0" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="32">
+    <format dxfId="30">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="50">
@@ -11751,7 +11787,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="31">
+    <format dxfId="29">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="50">
@@ -11809,7 +11845,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="30">
+    <format dxfId="28">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="50">
@@ -11867,7 +11903,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="29">
+    <format dxfId="27">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="50">
@@ -11925,7 +11961,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="28">
+    <format dxfId="26">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="50">
@@ -11983,7 +12019,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="27">
+    <format dxfId="25">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="50">
@@ -12041,7 +12077,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="26">
+    <format dxfId="24">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="50">
@@ -12099,7 +12135,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="25">
+    <format dxfId="23">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="50">
@@ -12157,7 +12193,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="24">
+    <format dxfId="22">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="50">
@@ -12215,7 +12251,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="23">
+    <format dxfId="21">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="50">
@@ -12273,7 +12309,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="22">
+    <format dxfId="20">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="39">
@@ -12320,22 +12356,22 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="21">
+    <format dxfId="19">
       <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="20">
+    <format dxfId="18">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
     </format>
-    <format dxfId="18">
+    <format dxfId="17">
       <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="17">
+    <format dxfId="16">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="16">
+    <format dxfId="15">
       <pivotArea field="0" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="15">
+    <format dxfId="14">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="50">
@@ -12393,7 +12429,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="14">
+    <format dxfId="13">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="50">
@@ -12451,7 +12487,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="13">
+    <format dxfId="12">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="50">
@@ -12509,7 +12545,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="12">
+    <format dxfId="11">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="50">
@@ -12567,7 +12603,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="11">
+    <format dxfId="10">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="50">
@@ -12625,7 +12661,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="10">
+    <format dxfId="9">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="50">
@@ -12683,7 +12719,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="9">
+    <format dxfId="8">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="50">
@@ -12741,7 +12777,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="8">
+    <format dxfId="7">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="50">
@@ -12799,7 +12835,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="7">
+    <format dxfId="6">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="50">
@@ -12857,7 +12893,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="6">
+    <format dxfId="5">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="50">
@@ -12915,7 +12951,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="5">
+    <format dxfId="4">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="39">
@@ -12962,10 +12998,10 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="4">
+    <format dxfId="3">
       <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="3">
+    <format dxfId="2">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
     </format>
   </formats>
@@ -13248,7 +13284,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A355" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B359" sqref="B359"/>
+      <selection pane="bottomLeft" activeCell="B364" sqref="B364"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -22212,16 +22248,16 @@
         <v/>
       </c>
     </row>
-    <row r="367" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="367" spans="1:9" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A367" s="1" t="s">
         <v>1851</v>
       </c>
       <c r="B367" s="2" t="s">
-        <v>1857</v>
+        <v>1861</v>
       </c>
       <c r="C367">
         <f t="shared" si="10"/>
-        <v>62</v>
+        <v>139</v>
       </c>
       <c r="D367" t="s">
         <v>1853</v>
@@ -22265,10 +22301,10 @@
     </row>
     <row r="369" spans="1:9" ht="27" x14ac:dyDescent="0.15">
       <c r="A369" s="1" t="s">
+        <v>1857</v>
+      </c>
+      <c r="B369" s="2" t="s">
         <v>1858</v>
-      </c>
-      <c r="B369" s="2" t="s">
-        <v>1859</v>
       </c>
       <c r="C369">
         <f t="shared" si="10"/>
@@ -22290,10 +22326,10 @@
     </row>
     <row r="370" spans="1:9" ht="27" x14ac:dyDescent="0.15">
       <c r="A370" s="1" t="s">
+        <v>1859</v>
+      </c>
+      <c r="B370" s="2" t="s">
         <v>1860</v>
-      </c>
-      <c r="B370" s="2" t="s">
-        <v>1861</v>
       </c>
       <c r="C370">
         <f t="shared" si="10"/>
@@ -29961,7 +29997,7 @@
       </c>
       <c r="G82" s="5" t="str">
         <f ca="1">OFFSET(todayssatellite!$B$1,MATCH(B82&amp;"_"&amp;C82,todayssatellite!$G:$G,0)-1,0)</f>
-        <v>【今日の人工衛星】8/27 2023年：X線天文衛星代替機(XRISM)、小型月着陸実証機(SLIM)が打ち上げられました。</v>
+        <v>【今日の人工衛星】8/27 2023年：X線天文衛星代替機(XRISM)、小型月着陸実証機(SLIM) XRISMは、喪失したASTRO-Hの代替機として、期待された科学的成果を上げている。SLIMは、日本発の月面探査機として、ピンポイント着陸を含む様々な世界初の成果を上げた。</v>
       </c>
       <c r="H82" s="6" t="s">
         <v>1657</v>

</xml_diff>